<commit_message>
Fixed format error in timesheet
</commit_message>
<xml_diff>
--- a/man/completed sheets/2015-11-9/Joshua Doyle.xlsx
+++ b/man/completed sheets/2015-11-9/Joshua Doyle.xlsx
@@ -49,12 +49,6 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>abc123</t>
-  </si>
-  <si>
-    <t>John Smith</t>
-  </si>
-  <si>
     <t>Time Budgeted</t>
   </si>
   <si>
@@ -74,6 +68,12 @@
   </si>
   <si>
     <t>Ongoing Task.</t>
+  </si>
+  <si>
+    <t>Joshua Doyle</t>
+  </si>
+  <si>
+    <t>jod32</t>
   </si>
 </sst>
 </file>
@@ -474,7 +474,7 @@
       <pane xSplit="8" ySplit="2" topLeftCell="I3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -484,7 +484,7 @@
     <col min="3" max="3" width="36.26953125" customWidth="1"/>
     <col min="4" max="4" width="24" customWidth="1"/>
     <col min="5" max="5" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.90625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.453125" customWidth="1"/>
     <col min="8" max="8" width="68.54296875" customWidth="1"/>
   </cols>
@@ -494,19 +494,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="8">
-        <v>0</v>
+        <v>42327</v>
       </c>
       <c r="G1" s="4" t="str">
         <f>"Total hours accounted this week: " &amp;TEXT(I1, "hh:mm")</f>
@@ -547,7 +547,7 @@
         <v>8</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>9</v>
@@ -555,28 +555,28 @@
     </row>
     <row r="3" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="D3" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="E3" s="10" t="s">
         <v>15</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>17</v>
       </c>
       <c r="F3" s="11">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.35">

</xml_diff>